<commit_message>
updated new metatable given
</commit_message>
<xml_diff>
--- a/src-data/metatable.xlsx
+++ b/src-data/metatable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="166">
   <si>
     <t>Series</t>
   </si>
@@ -480,6 +480,48 @@
   </si>
   <si>
     <t>Tax Foundation</t>
+  </si>
+  <si>
+    <t>Source Link</t>
+  </si>
+  <si>
+    <t>http://www.census.gov/acs/www/</t>
+  </si>
+  <si>
+    <t>http://www.nsf.gov/statistics/seind14/</t>
+  </si>
+  <si>
+    <t>http://www.nsf.gov/statistics/srvygradpostdoc/</t>
+  </si>
+  <si>
+    <t>http://nces.ed.gov/nationsreportcard/</t>
+  </si>
+  <si>
+    <t>http://www.census.gov/ces/dataproducts/bds/</t>
+  </si>
+  <si>
+    <t>http://www.kauffman.org/what-we-do/research/kauffman-index-of-entrepreneurial-activity</t>
+  </si>
+  <si>
+    <t>http://www.uspto.gov/learning-and-resources/statistics</t>
+  </si>
+  <si>
+    <t>http://www.nsf.gov/statistics/srvyherd/</t>
+  </si>
+  <si>
+    <t>http://www.autm.net/Home.htm</t>
+  </si>
+  <si>
+    <t>http://bea.gov/regional/index.htm</t>
+  </si>
+  <si>
+    <t>http://www.bls.gov/sae/</t>
+  </si>
+  <si>
+    <t>http://www.bls.gov/lau/</t>
+  </si>
+  <si>
+    <t>http://taxfoundation.org/tax-topics/tax-burdens</t>
   </si>
 </sst>
 </file>
@@ -1000,11 +1042,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1013,13 +1055,13 @@
     <col min="2" max="2" width="36.875" style="4" customWidth="1"/>
     <col min="3" max="3" width="53" style="7" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="26.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="26.625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="11" style="4"/>
+    <col min="5" max="6" width="26.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1036,16 +1078,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1062,13 +1107,16 @@
         <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1085,10 +1133,13 @@
         <v>134</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1105,13 +1156,16 @@
         <v>135</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1127,11 +1181,14 @@
       <c r="E5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1148,10 +1205,13 @@
         <v>24</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1168,10 +1228,13 @@
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1188,10 +1251,13 @@
         <v>24</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1208,10 +1274,13 @@
         <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1228,10 +1297,13 @@
         <v>97</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1248,10 +1320,13 @@
         <v>97</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1268,10 +1343,13 @@
         <v>97</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1288,10 +1366,13 @@
         <v>97</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
@@ -1308,10 +1389,13 @@
         <v>97</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -1328,10 +1412,13 @@
         <v>34</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1348,10 +1435,13 @@
         <v>36</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1368,10 +1458,13 @@
         <v>38</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1388,16 +1481,19 @@
         <v>131</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="I18" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -1414,10 +1510,13 @@
         <v>46</v>
       </c>
       <c r="F19" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -1434,13 +1533,16 @@
         <v>121</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
@@ -1457,10 +1559,13 @@
         <v>48</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
@@ -1477,10 +1582,13 @@
         <v>49</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -1497,13 +1605,16 @@
         <v>126</v>
       </c>
       <c r="F23" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>44</v>
       </c>
@@ -1520,10 +1631,13 @@
         <v>53</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>44</v>
       </c>
@@ -1540,10 +1654,13 @@
         <v>56</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -1560,11 +1677,14 @@
         <v>149</v>
       </c>
       <c r="F26" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
@@ -1581,11 +1701,14 @@
         <v>149</v>
       </c>
       <c r="F27" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1602,11 +1725,14 @@
         <v>149</v>
       </c>
       <c r="F28" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>63</v>
       </c>
@@ -1623,10 +1749,13 @@
         <v>66</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>63</v>
       </c>
@@ -1643,13 +1772,16 @@
         <v>66</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>63</v>
       </c>
@@ -1666,13 +1798,16 @@
         <v>66</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="I31" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>63</v>
       </c>
@@ -1689,10 +1824,13 @@
         <v>66</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
@@ -1709,13 +1847,16 @@
         <v>75</v>
       </c>
       <c r="F33" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>63</v>
       </c>
@@ -1732,13 +1873,16 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="I34" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>63</v>
       </c>
@@ -1755,10 +1899,13 @@
         <v>151</v>
       </c>
       <c r="F35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>63</v>
       </c>
@@ -1775,6 +1922,9 @@
         <v>75</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>